<commit_message>
Process Python / CC File
</commit_message>
<xml_diff>
--- a/src/m3c2_stats_all.xlsx
+++ b/src/m3c2_stats_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1e42ad97154f173/09 Sonstiges/M3C2_Project/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_912932CA9756DE0F62355476585DCE3A0742BC89" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7A497F1-7D12-4727-821E-5BD976A6BFFF}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_FD0111A49074300F62355476585DCE3A07437AE8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3372166A-7645-4146-B2A6-DEC4B7DFE2DC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
   <si>
     <t>Timestamp</t>
   </si>
@@ -205,55 +205,85 @@
     <t>Params Path</t>
   </si>
   <si>
-    <t>2025-08-19 16:07:00</t>
-  </si>
-  <si>
     <t>data\rocks</t>
   </si>
   <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>data\rocks\points_80_m3c2_distances.txt</t>
-  </si>
-  <si>
-    <t>data\rocks\points_80_m3c2_params.txt</t>
-  </si>
-  <si>
-    <t>2025-08-19 16:12:21</t>
-  </si>
-  <si>
-    <t>2025-08-19 16:13:20</t>
-  </si>
-  <si>
-    <t>2025-08-19 16:14:03</t>
-  </si>
-  <si>
-    <t>data\rocks\points_40_m3c2_distances.txt</t>
-  </si>
-  <si>
-    <t>data\rocks\points_40_m3c2_params.txt</t>
-  </si>
-  <si>
-    <t>2025-08-19 16:14:37</t>
-  </si>
-  <si>
-    <t>data\rocks\points_overlap2_m3c2_distances.txt</t>
-  </si>
-  <si>
-    <t>data\rocks\points_overlap2_m3c2_params.txt</t>
-  </si>
-  <si>
-    <t>2025-08-19 16:15:34</t>
-  </si>
-  <si>
-    <t>data\rocks\points_zshift_m3c2_distances.txt</t>
-  </si>
-  <si>
-    <t>data\rocks\points_zshift_m3c2_params.txt</t>
-  </si>
-  <si>
-    <t>2025-08-20 09:38:42</t>
+    <t>2025-08-20 10:25:42</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>data\rocks\python_points_zshift_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\rocks\python_points_zshift_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:31:22</t>
+  </si>
+  <si>
+    <t>data\rocks\python_points_40_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\rocks\python_points_40_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:31:54</t>
+  </si>
+  <si>
+    <t>data\rocks\python_points_80_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\rocks\python_points_80_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:32:19</t>
+  </si>
+  <si>
+    <t>data\rocks\python_points_overlap2_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\rocks\python_points_overlap2_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>data\rocks\CC_points_40_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\rocks\CC_points_40_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:49:31</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:50:17</t>
+  </si>
+  <si>
+    <t>data\rocks\CC_points_80_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\rocks\CC_points_80_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:50:35</t>
+  </si>
+  <si>
+    <t>data\rocks\CC_points_overlap2_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\rocks\CC_points_overlap2_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:50:52</t>
+  </si>
+  <si>
+    <t>data\rocks\CC_points_zshift_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\rocks\CC_points_zshift_m3c2_params.txt</t>
   </si>
 </sst>
 </file>
@@ -616,18 +646,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI8"/>
+  <dimension ref="A1:BI9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="BH2" sqref="BH2:BH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="41" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="47.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.3">
@@ -817,10 +846,10 @@
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -829,163 +858,163 @@
         <v>474380</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>5124</v>
       </c>
       <c r="G2">
-        <v>2.108014671782115E-6</v>
+        <v>1.080146717821156E-2</v>
       </c>
       <c r="H2">
-        <v>0.99999789198532818</v>
+        <v>0.98919853282178849</v>
       </c>
       <c r="I2">
-        <v>474379</v>
+        <v>469256</v>
       </c>
       <c r="J2">
-        <v>1.941444999999995</v>
+        <v>542.06407400000001</v>
       </c>
       <c r="K2">
-        <v>17.826035987455001</v>
+        <v>574.12937721256196</v>
       </c>
       <c r="L2">
-        <v>2.3130931678366822</v>
+        <v>2.313093168488944</v>
       </c>
       <c r="M2">
-        <v>1.1565465839183411</v>
+        <v>1.156546584244472</v>
       </c>
       <c r="N2">
-        <v>-0.14627200000000001</v>
+        <v>-0.15721199999999999</v>
       </c>
       <c r="O2">
-        <v>8.8577000000000003E-2</v>
+        <v>1.656102</v>
       </c>
       <c r="P2">
-        <v>4.09260317172555E-6</v>
+        <v>1.155156405032647E-3</v>
       </c>
       <c r="Q2">
-        <v>3.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>6.1300591037489324E-3</v>
+        <v>3.4978402234350753E-2</v>
       </c>
       <c r="S2">
-        <v>6.1300577375791847E-3</v>
+        <v>3.495932259852793E-2</v>
       </c>
       <c r="T2">
-        <v>4.2637385824414661E-3</v>
+        <v>1.3344316023662991E-3</v>
       </c>
       <c r="U2">
-        <v>3.9311546219027516E-3</v>
+        <v>2.0914181288734509E-4</v>
       </c>
       <c r="V2">
-        <v>4.5011736E-3</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>4.4107349999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>7634</v>
+        <v>843</v>
       </c>
       <c r="Y2">
-        <v>466745</v>
+        <v>468413</v>
       </c>
       <c r="Z2">
-        <v>-4.2287201791127921E-6</v>
+        <v>5.6942305187943098E-5</v>
       </c>
       <c r="AA2">
-        <v>5.2367476220633209E-3</v>
+        <v>3.1879620835603092E-3</v>
       </c>
       <c r="AB2">
-        <v>5.1286075451925585E-4</v>
+        <v>0.61137788612099653</v>
       </c>
       <c r="AC2">
-        <v>2.5654202285651941E-2</v>
+        <v>0.54920229863782977</v>
       </c>
       <c r="AD2">
-        <v>3902</v>
+        <v>788</v>
       </c>
       <c r="AE2">
-        <v>3732</v>
+        <v>55</v>
       </c>
       <c r="AF2">
-        <v>234520</v>
+        <v>2675</v>
       </c>
       <c r="AG2">
-        <v>232123</v>
+        <v>1690</v>
       </c>
       <c r="AH2">
-        <v>-9.3640000000000008E-3</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>-3.016E-3</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>3.0569999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>9.2049999999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>4.09260317172555E-6</v>
+        <v>1.155156405032647E-3</v>
       </c>
       <c r="AM2">
-        <v>6.1300577375791847E-3</v>
+        <v>3.495932259852793E-2</v>
       </c>
       <c r="AN2">
-        <v>32994274243748.09</v>
+        <v>1110220780587.2539</v>
       </c>
       <c r="AO2">
-        <v>13.82314781793478</v>
+        <v>2.554092792412249</v>
       </c>
       <c r="AP2">
-        <v>0.1124207329376318</v>
+        <v>0.17201232947294931</v>
       </c>
       <c r="AQ2">
-        <v>-0.1096417896098531</v>
+        <v>-0.1572143602249286</v>
       </c>
       <c r="AR2">
-        <v>2.1698868973674822E-3</v>
+        <v>-1.560775682153898E-2</v>
       </c>
       <c r="AS2">
-        <v>-0.76084995647421572</v>
+        <v>0.33491757138315947</v>
       </c>
       <c r="AT2">
-        <v>14758002864334.789</v>
+        <v>177850614920.15961</v>
       </c>
       <c r="AU2">
-        <v>-6.1205945124484129E-2</v>
+        <v>35.543475564065872</v>
       </c>
       <c r="AV2">
-        <v>7.9848090773539164</v>
+        <v>1328.9798467837591</v>
       </c>
       <c r="AW2">
-        <v>8.5033275081738441E-2</v>
+        <v>7.2561672093697264E-3</v>
       </c>
       <c r="AX2">
-        <v>0.94784339104386994</v>
+        <v>0.99756849139915105</v>
       </c>
       <c r="AY2">
-        <v>0.14627200000000001</v>
+        <v>1.656102</v>
       </c>
       <c r="AZ2">
-        <v>4.09260317172555E-6</v>
+        <v>1.155156405032647E-3</v>
       </c>
       <c r="BA2">
-        <v>0.91496672491826159</v>
+        <v>0.99274383279063028</v>
       </c>
       <c r="BC2">
-        <v>1.335257031087538E-3</v>
+        <v>6.6013667247068322E-2</v>
       </c>
       <c r="BD2">
-        <v>-1.201082056248348E-2</v>
+        <v>-6.7365115888082083E-2</v>
       </c>
       <c r="BE2">
-        <v>1.201900576882693E-2</v>
+        <v>6.9675428698147385E-2</v>
       </c>
       <c r="BF2">
-        <v>0.91495829284179953</v>
+        <v>0.99274383279063028</v>
       </c>
       <c r="BG2">
-        <v>0.91495829284179953</v>
+        <v>0.99274383279063028</v>
       </c>
       <c r="BH2" t="s">
         <v>64</v>
@@ -999,180 +1028,186 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
       </c>
       <c r="E3">
-        <v>48</v>
+        <v>474380</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>6.3240440153463467E-6</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0.99999367595598465</v>
       </c>
       <c r="I3">
-        <v>48</v>
+        <v>474377</v>
       </c>
       <c r="J3">
-        <v>1.1318E-2</v>
+        <v>154.524157</v>
       </c>
       <c r="K3">
-        <v>2.7922134799999998E-4</v>
+        <v>109.503050332033</v>
       </c>
       <c r="L3">
-        <v>82.338734504234154</v>
+        <v>2.313093165601074</v>
       </c>
       <c r="M3">
-        <v>41.169367252117077</v>
+        <v>1.156546582800537</v>
       </c>
       <c r="N3">
-        <v>-4.829E-3</v>
+        <v>-0.26206699999999999</v>
       </c>
       <c r="O3">
-        <v>5.1500000000000001E-3</v>
+        <v>0.22663700000000001</v>
       </c>
       <c r="P3">
-        <v>2.357916666666667E-4</v>
+        <v>3.2574125010276629E-4</v>
       </c>
       <c r="Q3">
-        <v>-4.6E-5</v>
+        <v>1.01E-4</v>
       </c>
       <c r="R3">
-        <v>2.4118688639033982E-3</v>
+        <v>1.519327142252982E-2</v>
       </c>
       <c r="S3">
-        <v>2.400315334825244E-3</v>
+        <v>1.5189779101640769E-2</v>
       </c>
       <c r="T3">
-        <v>1.916708333333333E-3</v>
+        <v>1.0523272420458829E-2</v>
       </c>
       <c r="U3">
-        <v>1.916708333333333E-3</v>
+        <v>9.6918633950720447E-3</v>
       </c>
       <c r="V3">
-        <v>2.4114488999999999E-3</v>
+        <v>1.1070574200000001E-2</v>
       </c>
       <c r="W3">
-        <v>2.4114488999999999E-3</v>
+        <v>1.0845219E-2</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>7571</v>
       </c>
       <c r="Y3">
-        <v>48</v>
+        <v>466806</v>
       </c>
       <c r="Z3">
-        <v>2.357916666666667E-4</v>
+        <v>2.4363661563904491E-4</v>
       </c>
       <c r="AA3">
-        <v>2.400315334825244E-3</v>
+        <v>1.29198016672593E-2</v>
+      </c>
+      <c r="AB3">
+        <v>5.3880759476951524E-3</v>
+      </c>
+      <c r="AC3">
+        <v>6.4334365556486098E-2</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <v>4177</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>3394</v>
       </c>
       <c r="AF3">
-        <v>24</v>
+        <v>234704</v>
       </c>
       <c r="AG3">
-        <v>24</v>
+        <v>232076</v>
       </c>
       <c r="AH3">
-        <v>-3.8297000000000001E-3</v>
+        <v>-2.2290000000000001E-2</v>
       </c>
       <c r="AI3">
-        <v>-1.121E-3</v>
+        <v>-7.2179999999999996E-3</v>
       </c>
       <c r="AJ3">
-        <v>1.8894999999999999E-3</v>
+        <v>7.7320000000000002E-3</v>
       </c>
       <c r="AK3">
-        <v>4.8698499999999994E-3</v>
+        <v>2.3505000000000002E-2</v>
       </c>
       <c r="AL3">
-        <v>2.357916666666667E-4</v>
+        <v>3.2574125010276629E-4</v>
       </c>
       <c r="AM3">
-        <v>2.400315334825244E-3</v>
+        <v>1.5189779101640769E-2</v>
       </c>
       <c r="AN3">
-        <v>352.37616317732522</v>
+        <v>20151777901228.859</v>
       </c>
       <c r="AO3">
-        <v>3.0862312297452439</v>
+        <v>0.16922327411571639</v>
       </c>
       <c r="AP3">
-        <v>7.5422880045705343E-3</v>
+        <v>2.8996241196366291E-3</v>
       </c>
       <c r="AQ3">
-        <v>-6.5074699520993274E-3</v>
+        <v>-0.12792000000000001</v>
       </c>
       <c r="AR3">
-        <v>1.3605171745745531E-4</v>
+        <v>-0.12792000000000001</v>
       </c>
       <c r="AS3">
-        <v>0.140660342983085</v>
+        <v>549.8884461550665</v>
       </c>
       <c r="AT3">
-        <v>338.62854132669418</v>
+        <v>29154900.213798359</v>
       </c>
       <c r="AU3">
-        <v>7.5612881842482438E-2</v>
+        <v>-1.272125943096011E-2</v>
       </c>
       <c r="AV3">
-        <v>-0.23111564637580881</v>
+        <v>7.9371765396027163</v>
       </c>
       <c r="AW3">
-        <v>0</v>
+        <v>0.38149193573887441</v>
       </c>
       <c r="AX3">
-        <v>0.91666666666666663</v>
+        <v>0.94863578967783013</v>
       </c>
       <c r="AY3">
-        <v>5.1500000000000001E-3</v>
+        <v>0.26206699999999999</v>
       </c>
       <c r="AZ3">
-        <v>2.357916666666667E-4</v>
+        <v>3.2574125010276629E-4</v>
       </c>
       <c r="BA3">
-        <v>1</v>
+        <v>0.61850806426112559</v>
       </c>
       <c r="BC3">
-        <v>0.19458948360604661</v>
+        <v>4.2869816020287319E-2</v>
       </c>
       <c r="BD3">
-        <v>-4.4688263895908114E-3</v>
+        <v>-2.9446225789113149E-2</v>
       </c>
       <c r="BE3">
-        <v>4.9404097229241439E-3</v>
+        <v>3.0097708289318681E-2</v>
       </c>
       <c r="BF3">
-        <v>1</v>
+        <v>0.61845957961705567</v>
       </c>
       <c r="BG3">
-        <v>1</v>
+        <v>0.61845957961705567</v>
       </c>
       <c r="BH3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="BI3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
@@ -1199,10 +1234,10 @@
         <v>17.826007639863999</v>
       </c>
       <c r="L4">
-        <v>2.3130931643851289</v>
+        <v>2.3130931637459531</v>
       </c>
       <c r="M4">
-        <v>1.1565465821925649</v>
+        <v>1.1565465818729761</v>
       </c>
       <c r="N4">
         <v>-0.14627200000000001</v>
@@ -1340,18 +1375,18 @@
         <v>0.91495829284179953</v>
       </c>
       <c r="BH4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="BI4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
@@ -1360,586 +1395,586 @@
         <v>474380</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>337467</v>
       </c>
       <c r="G5">
-        <v>6.3240440153463467E-6</v>
+        <v>0.71138538724229516</v>
       </c>
       <c r="H5">
-        <v>0.99999367595598465</v>
+        <v>0.28861461275770478</v>
       </c>
       <c r="I5">
-        <v>474377</v>
+        <v>136913</v>
       </c>
       <c r="J5">
-        <v>154.51543599999999</v>
+        <v>-270.12283400000013</v>
       </c>
       <c r="K5">
-        <v>109.503596954142</v>
+        <v>95.293457053468003</v>
       </c>
       <c r="L5">
-        <v>2.3130931678366822</v>
+        <v>2.313093166035916</v>
       </c>
       <c r="M5">
-        <v>1.1565465839183411</v>
+        <v>1.156546583017958</v>
       </c>
       <c r="N5">
-        <v>-0.26206699999999999</v>
+        <v>-1.130681</v>
       </c>
       <c r="O5">
-        <v>0.22663700000000001</v>
+        <v>0.46836</v>
       </c>
       <c r="P5">
-        <v>3.2572286599055192E-4</v>
+        <v>-1.9729524150372871E-3</v>
       </c>
       <c r="Q5">
-        <v>1.01E-4</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>1.519330934370041E-2</v>
+        <v>2.6382090022254549E-2</v>
       </c>
       <c r="S5">
-        <v>1.5189817425760751E-2</v>
+        <v>2.6308214168018731E-2</v>
       </c>
       <c r="T5">
-        <v>1.052328973790888E-2</v>
+        <v>3.9128609993207362E-3</v>
       </c>
       <c r="U5">
-        <v>9.6918039395464881E-3</v>
+        <v>1.7134158666291921E-3</v>
       </c>
       <c r="V5">
-        <v>1.1070574200000001E-2</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>1.0845219E-2</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>7572</v>
+        <v>1711</v>
       </c>
       <c r="Y5">
-        <v>466805</v>
+        <v>135202</v>
       </c>
       <c r="Z5">
-        <v>2.4371678109703191E-4</v>
+        <v>-4.194123015931718E-4</v>
       </c>
       <c r="AA5">
-        <v>1.2919686548739529E-2</v>
+        <v>8.1064992861220458E-3</v>
       </c>
       <c r="AB5">
-        <v>5.3813026941362911E-3</v>
+        <v>-0.1247325844535359</v>
       </c>
       <c r="AC5">
-        <v>6.433279341472356E-2</v>
+        <v>0.18689489481963709</v>
       </c>
       <c r="AD5">
-        <v>4177</v>
+        <v>319</v>
       </c>
       <c r="AE5">
-        <v>3395</v>
+        <v>1392</v>
       </c>
       <c r="AF5">
-        <v>234703</v>
+        <v>4870</v>
       </c>
       <c r="AG5">
-        <v>232076</v>
+        <v>7539</v>
       </c>
       <c r="AH5">
-        <v>-2.2290000000000001E-2</v>
+        <v>-4.8277999999999993E-3</v>
       </c>
       <c r="AI5">
-        <v>-7.2179999999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
-        <v>7.7320000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="AK5">
-        <v>2.3505000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="AL5">
-        <v>3.2572286599055192E-4</v>
+        <v>-1.9729524150372871E-3</v>
       </c>
       <c r="AM5">
-        <v>1.5189817425760751E-2</v>
+        <v>2.6308214168018731E-2</v>
       </c>
       <c r="AN5">
-        <v>20148153107731.309</v>
+        <v>118150822930589</v>
       </c>
       <c r="AO5">
-        <v>11.126978188870829</v>
+        <v>471949102.92391568</v>
       </c>
       <c r="AP5">
-        <v>0.22003451349229511</v>
+        <v>25505311.94613266</v>
       </c>
       <c r="AQ5">
-        <v>-0.21307153483903679</v>
+        <v>-25505311.940391649</v>
       </c>
       <c r="AR5">
-        <v>5.1086440801866029E-3</v>
-      </c>
-      <c r="AS5">
-        <v>-0.68166729940940785</v>
+        <v>5.7410076260566711E-3</v>
       </c>
       <c r="AT5">
-        <v>14774066340089.23</v>
+        <v>316265324530.12549</v>
       </c>
       <c r="AU5">
-        <v>-1.2735665345618961E-2</v>
+        <v>-15.016896742700609</v>
       </c>
       <c r="AV5">
-        <v>7.9371323232466962</v>
+        <v>413.95897101341183</v>
       </c>
       <c r="AW5">
-        <v>0.38149193573887441</v>
+        <v>6.1221359549494932E-2</v>
       </c>
       <c r="AX5">
-        <v>0.94863578967783013</v>
+        <v>0.97962209578345372</v>
       </c>
       <c r="AY5">
-        <v>0.26206699999999999</v>
+        <v>1.130681</v>
       </c>
       <c r="AZ5">
-        <v>3.2572286599055192E-4</v>
+        <v>-1.9729524150372871E-3</v>
       </c>
       <c r="BA5">
-        <v>0.61850806426112559</v>
+        <v>0.93877864045050508</v>
       </c>
       <c r="BC5">
-        <v>4.2867290711641651E-2</v>
+        <v>-0.14914873671876189</v>
       </c>
       <c r="BD5">
-        <v>-2.9446319288500521E-2</v>
+        <v>-5.3537052184353999E-2</v>
       </c>
       <c r="BE5">
-        <v>3.0097765020481629E-2</v>
+        <v>4.959114735427942E-2</v>
       </c>
       <c r="BF5">
-        <v>0.61845957961705567</v>
+        <v>0.9387713365421837</v>
       </c>
       <c r="BG5">
-        <v>0.61845957961705567</v>
+        <v>0.9387713365421837</v>
       </c>
       <c r="BH5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="BI5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E6">
         <v>474380</v>
       </c>
       <c r="F6">
-        <v>337467</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>0.71138538724229516</v>
+        <v>6.3240440153463467E-6</v>
       </c>
       <c r="H6">
-        <v>0.28861461275770478</v>
+        <v>0.99999367595598465</v>
       </c>
       <c r="I6">
-        <v>136913</v>
+        <v>474377</v>
       </c>
       <c r="J6">
-        <v>-270.12283400000013</v>
+        <v>157.56662600000001</v>
       </c>
       <c r="K6">
-        <v>95.293457053468003</v>
+        <v>106.75045038149599</v>
       </c>
       <c r="L6">
-        <v>2.313093166344935</v>
+        <v>4.9174119999999997</v>
       </c>
       <c r="M6">
-        <v>1.1565465831724671</v>
+        <v>2.4587059999999998</v>
       </c>
       <c r="N6">
-        <v>-1.130681</v>
+        <v>-0.54669299999999998</v>
       </c>
       <c r="O6">
-        <v>0.46836</v>
+        <v>0.43005399999999999</v>
       </c>
       <c r="P6">
-        <v>-1.9729524150372871E-3</v>
+        <v>3.3215485995315971E-4</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>9.2E-5</v>
       </c>
       <c r="R6">
-        <v>2.6382090022254549E-2</v>
+        <v>1.50010979178776E-2</v>
       </c>
       <c r="S6">
-        <v>2.6308214168018731E-2</v>
+        <v>1.4997420174508721E-2</v>
       </c>
       <c r="T6">
-        <v>3.9128609993207362E-3</v>
+        <v>1.026142670070429E-2</v>
       </c>
       <c r="U6">
-        <v>1.7134158666291921E-3</v>
+        <v>9.4495244585583518E-3</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1.07592282E-2</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>1.05501816E-2</v>
       </c>
       <c r="X6">
-        <v>1711</v>
+        <v>7383</v>
       </c>
       <c r="Y6">
-        <v>135202</v>
+        <v>466994</v>
       </c>
       <c r="Z6">
-        <v>-4.194123015931718E-4</v>
+        <v>2.6760615553947148E-4</v>
       </c>
       <c r="AA6">
-        <v>8.1064992861220458E-3</v>
+        <v>1.2622828788120211E-2</v>
       </c>
       <c r="AB6">
-        <v>-0.1247325844535359</v>
+        <v>4.4150287146146553E-3</v>
       </c>
       <c r="AC6">
-        <v>0.18689489481963709</v>
+        <v>6.6003982074430104E-2</v>
       </c>
       <c r="AD6">
-        <v>319</v>
+        <v>4004</v>
       </c>
       <c r="AE6">
-        <v>1392</v>
+        <v>3379</v>
       </c>
       <c r="AF6">
-        <v>4870</v>
+        <v>234882</v>
       </c>
       <c r="AG6">
-        <v>7539</v>
+        <v>232088</v>
       </c>
       <c r="AH6">
-        <v>-4.8277999999999993E-3</v>
+        <v>-2.1680999999999999E-2</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>-6.999E-3</v>
       </c>
       <c r="AJ6">
-        <v>0</v>
+        <v>7.5230000000000002E-3</v>
       </c>
       <c r="AK6">
-        <v>0</v>
+        <v>2.3002199999999959E-2</v>
       </c>
       <c r="AL6">
-        <v>-1.9729524150372871E-3</v>
+        <v>3.3215485995315971E-4</v>
       </c>
       <c r="AM6">
-        <v>2.6308214168018731E-2</v>
+        <v>1.4997420174508721E-2</v>
       </c>
       <c r="AN6">
-        <v>118150822930589</v>
+        <v>35348281676587.977</v>
       </c>
       <c r="AO6">
-        <v>471949102.92391568</v>
+        <v>16.90564866585245</v>
       </c>
       <c r="AP6">
-        <v>25505311.94613266</v>
+        <v>0.55339832002593758</v>
       </c>
       <c r="AQ6">
-        <v>-25505311.940391649</v>
+        <v>-0.54679544064698882</v>
       </c>
       <c r="AR6">
-        <v>5.7410076260566711E-3</v>
+        <v>4.610536125178033E-3</v>
+      </c>
+      <c r="AS6">
+        <v>-0.82318445709373689</v>
       </c>
       <c r="AT6">
-        <v>316265324530.12549</v>
+        <v>137132641585.59711</v>
       </c>
       <c r="AU6">
-        <v>-15.016896742700609</v>
+        <v>-0.283607753450343</v>
       </c>
       <c r="AV6">
-        <v>413.95897101341183</v>
+        <v>28.29928954371081</v>
       </c>
       <c r="AW6">
-        <v>6.1221359549494932E-2</v>
+        <v>0.36936234260935918</v>
       </c>
       <c r="AX6">
-        <v>0.97962209578345372</v>
+        <v>0.95015989392403088</v>
       </c>
       <c r="AY6">
-        <v>1.130681</v>
+        <v>0.54669299999999998</v>
       </c>
       <c r="AZ6">
-        <v>-1.9729524150372871E-3</v>
+        <v>3.3215485995315971E-4</v>
       </c>
       <c r="BA6">
-        <v>0.93877864045050508</v>
+        <v>0.63063765739064082</v>
       </c>
       <c r="BC6">
-        <v>-0.14914873671876189</v>
+        <v>4.4273216406237978E-2</v>
       </c>
       <c r="BD6">
-        <v>-5.3537052184353999E-2</v>
+        <v>-2.9062788682083941E-2</v>
       </c>
       <c r="BE6">
-        <v>4.959114735427942E-2</v>
+        <v>2.9727098401990261E-2</v>
       </c>
       <c r="BF6">
-        <v>0.9387713365421837</v>
+        <v>0.63061657711061037</v>
       </c>
       <c r="BG6">
-        <v>0.9387713365421837</v>
+        <v>0.63061657711061037</v>
       </c>
       <c r="BH6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="BI6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E7">
         <v>474380</v>
       </c>
       <c r="F7">
-        <v>5124</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1.080146717821156E-2</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.98919853282178849</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>469256</v>
+        <v>474380</v>
       </c>
       <c r="J7">
-        <v>542.06398799999999</v>
+        <v>-0.32428499999999938</v>
       </c>
       <c r="K7">
-        <v>574.12936312758995</v>
+        <v>17.202745938214999</v>
       </c>
       <c r="L7">
-        <v>2.313093164075859</v>
+        <v>4.9174119999999997</v>
       </c>
       <c r="M7">
-        <v>1.156546582037929</v>
+        <v>2.4587059999999998</v>
       </c>
       <c r="N7">
-        <v>-0.15721199999999999</v>
+        <v>-0.261075</v>
       </c>
       <c r="O7">
-        <v>1.656102</v>
+        <v>0.11153100000000001</v>
       </c>
       <c r="P7">
-        <v>1.1551562217638131E-3</v>
+        <v>-6.8359753783886201E-7</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>2.0999999999999999E-5</v>
       </c>
       <c r="R7">
-        <v>3.4978401805292561E-2</v>
+        <v>6.0219299923444328E-3</v>
       </c>
       <c r="S7">
-        <v>3.4959322175291331E-2</v>
+        <v>6.0219299535441148E-3</v>
       </c>
       <c r="T7">
-        <v>1.334430728642788E-3</v>
+        <v>4.1487853092457517E-3</v>
       </c>
       <c r="U7">
-        <v>2.0914093759139899E-4</v>
+        <v>3.8324051374724602E-3</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>4.3721873999999997E-3</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>4.2861965999999993E-3</v>
       </c>
       <c r="X7">
-        <v>843</v>
+        <v>7341</v>
       </c>
       <c r="Y7">
-        <v>468413</v>
+        <v>467039</v>
       </c>
       <c r="Z7">
-        <v>5.6942121589281237E-5</v>
+        <v>-7.1357017294059032E-6</v>
       </c>
       <c r="AA7">
-        <v>3.187957370726423E-3</v>
+        <v>5.1189645374294613E-3</v>
       </c>
       <c r="AB7">
-        <v>0.61137788612099653</v>
+        <v>4.0980329655360332E-4</v>
       </c>
       <c r="AC7">
-        <v>0.54920229863782977</v>
+        <v>2.60020373053826E-2</v>
       </c>
       <c r="AD7">
-        <v>788</v>
+        <v>3739</v>
       </c>
       <c r="AE7">
-        <v>55</v>
+        <v>3602</v>
       </c>
       <c r="AF7">
-        <v>2675</v>
+        <v>234438</v>
       </c>
       <c r="AG7">
-        <v>1690</v>
+        <v>232519</v>
       </c>
       <c r="AH7">
-        <v>0</v>
+        <v>-9.1280500000000004E-3</v>
       </c>
       <c r="AI7">
-        <v>0</v>
+        <v>-2.934E-3</v>
       </c>
       <c r="AJ7">
-        <v>0</v>
+        <v>2.9640000000000001E-3</v>
       </c>
       <c r="AK7">
-        <v>0</v>
+        <v>8.9779999999999999E-3</v>
       </c>
       <c r="AL7">
-        <v>1.1551562217638131E-3</v>
+        <v>-6.8359753783886201E-7</v>
       </c>
       <c r="AM7">
-        <v>3.4959322175291331E-2</v>
+        <v>6.0219299535441148E-3</v>
       </c>
       <c r="AN7">
-        <v>1110220780594.072</v>
+        <v>5214335107057.4932</v>
       </c>
       <c r="AO7">
-        <v>2.5540927706881602</v>
+        <v>14.82266727439729</v>
       </c>
       <c r="AP7">
-        <v>0.1720123157814917</v>
+        <v>0.13408905138174179</v>
       </c>
       <c r="AQ7">
-        <v>-0.1572143600964393</v>
+        <v>-0.1314530437883894</v>
       </c>
       <c r="AR7">
-        <v>-1.560776850206216E-2</v>
+        <v>2.005635866599909E-3</v>
       </c>
       <c r="AS7">
-        <v>0.33491758073020322</v>
+        <v>-0.78361204942851848</v>
       </c>
       <c r="AT7">
-        <v>177850615518.90121</v>
+        <v>2135029892267.582</v>
       </c>
       <c r="AU7">
-        <v>35.543476859925953</v>
+        <v>-0.53783134443216274</v>
       </c>
       <c r="AV7">
-        <v>1328.9799120210171</v>
+        <v>28.942281980744671</v>
       </c>
       <c r="AW7">
-        <v>7.2561672093697264E-3</v>
+        <v>8.0125637674438213E-2</v>
       </c>
       <c r="AX7">
-        <v>0.99756849139915105</v>
+        <v>0.94859184619924952</v>
       </c>
       <c r="AY7">
-        <v>1.656102</v>
+        <v>0.261075</v>
       </c>
       <c r="AZ7">
-        <v>1.1551562217638131E-3</v>
+        <v>-6.8359753783886201E-7</v>
       </c>
       <c r="BA7">
-        <v>0.99274383279063028</v>
+        <v>0.91987436232556175</v>
       </c>
       <c r="BC7">
-        <v>6.6013657594112235E-2</v>
+        <v>-2.270360280851394E-4</v>
       </c>
       <c r="BD7">
-        <v>-6.7365115241807189E-2</v>
+        <v>-1.1803666306484301E-2</v>
       </c>
       <c r="BE7">
-        <v>6.9675427685334829E-2</v>
+        <v>1.1802299111408629E-2</v>
       </c>
       <c r="BF7">
-        <v>0.99274383279063028</v>
+        <v>0.91986171423753105</v>
       </c>
       <c r="BG7">
-        <v>0.99274383279063028</v>
+        <v>0.91986171423753105</v>
       </c>
       <c r="BH7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="BI7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E8">
         <v>474380</v>
       </c>
       <c r="F8">
-        <v>5124</v>
+        <v>337206</v>
       </c>
       <c r="G8">
-        <v>1.080146717821156E-2</v>
+        <v>0.71083519541296003</v>
       </c>
       <c r="H8">
-        <v>0.98919853282178849</v>
+        <v>0.28916480458704003</v>
       </c>
       <c r="I8">
-        <v>469256</v>
+        <v>137174</v>
       </c>
       <c r="J8">
-        <v>542.06398799999999</v>
+        <v>-313.62536799999998</v>
       </c>
       <c r="K8">
-        <v>574.12936312758995</v>
+        <v>126.260717360306</v>
       </c>
       <c r="L8">
-        <v>2.3130931661889149</v>
+        <v>4.9174119999999997</v>
       </c>
       <c r="M8">
-        <v>1.1565465830944579</v>
+        <v>2.4587059999999998</v>
       </c>
       <c r="N8">
-        <v>-0.15721199999999999</v>
+        <v>-1.340876</v>
       </c>
       <c r="O8">
-        <v>1.656102</v>
+        <v>0.49816899999999997</v>
       </c>
       <c r="P8">
-        <v>1.1551562217638131E-3</v>
+        <v>-2.2863324536719779E-3</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8">
-        <v>3.4978401805292561E-2</v>
+        <v>3.0338787830719E-2</v>
       </c>
       <c r="S8">
-        <v>3.4959322175291331E-2</v>
+        <v>3.025251610938616E-2</v>
       </c>
       <c r="T8">
-        <v>1.334430728642788E-3</v>
+        <v>4.3878391094522278E-3</v>
       </c>
       <c r="U8">
-        <v>2.0914093759139899E-4</v>
+        <v>2.0154777776138781E-3</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1948,37 +1983,37 @@
         <v>0</v>
       </c>
       <c r="X8">
-        <v>843</v>
+        <v>1590</v>
       </c>
       <c r="Y8">
-        <v>468413</v>
+        <v>135584</v>
       </c>
       <c r="Z8">
-        <v>5.6942121589281237E-5</v>
+        <v>-5.9403551303988664E-4</v>
       </c>
       <c r="AA8">
-        <v>3.187957370726423E-3</v>
+        <v>9.2267819613119379E-3</v>
       </c>
       <c r="AB8">
-        <v>0.61137788612099653</v>
+        <v>-0.14659349496855351</v>
       </c>
       <c r="AC8">
-        <v>0.54920229863782977</v>
+        <v>0.22501094820752049</v>
       </c>
       <c r="AD8">
-        <v>788</v>
+        <v>294</v>
       </c>
       <c r="AE8">
-        <v>55</v>
+        <v>1296</v>
       </c>
       <c r="AF8">
-        <v>2675</v>
+        <v>5144</v>
       </c>
       <c r="AG8">
-        <v>1690</v>
+        <v>8289</v>
       </c>
       <c r="AH8">
-        <v>0</v>
+        <v>-6.7964499999999964E-3</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -1990,73 +2025,252 @@
         <v>0</v>
       </c>
       <c r="AL8">
-        <v>1.1551562217638131E-3</v>
+        <v>-2.2863324536719779E-3</v>
       </c>
       <c r="AM8">
-        <v>3.4959322175291331E-2</v>
+        <v>3.025251610938616E-2</v>
       </c>
       <c r="AN8">
-        <v>1110220780594.072</v>
+        <v>64945070221820.68</v>
       </c>
       <c r="AO8">
-        <v>2.5540927706881602</v>
+        <v>26.276054919372381</v>
       </c>
       <c r="AP8">
-        <v>0.1720123157814917</v>
+        <v>1.3517148119654261</v>
       </c>
       <c r="AQ8">
-        <v>-0.1572143600964393</v>
+        <v>-1.3440239787421411</v>
       </c>
       <c r="AR8">
-        <v>-1.560776850206216E-2</v>
+        <v>5.696295141535801E-3</v>
       </c>
       <c r="AS8">
-        <v>0.33491758073020322</v>
+        <v>-0.92846182243001796</v>
       </c>
       <c r="AT8">
-        <v>177850615518.90121</v>
+        <v>2980962814372.395</v>
       </c>
       <c r="AU8">
-        <v>35.543476859925953</v>
+        <v>-16.906072943462188</v>
       </c>
       <c r="AV8">
-        <v>1328.9799120210171</v>
+        <v>496.83465113084162</v>
       </c>
       <c r="AW8">
-        <v>7.2561672093697264E-3</v>
+        <v>6.6958753116479794E-2</v>
       </c>
       <c r="AX8">
-        <v>0.99756849139915105</v>
+        <v>0.98120635105778065</v>
       </c>
       <c r="AY8">
-        <v>1.656102</v>
+        <v>1.340876</v>
       </c>
       <c r="AZ8">
-        <v>1.1551562217638131E-3</v>
+        <v>-2.2863324536719779E-3</v>
       </c>
       <c r="BA8">
-        <v>0.99274383279063028</v>
+        <v>0.93304124688352019</v>
       </c>
       <c r="BC8">
-        <v>6.6013657594112235E-2</v>
+        <v>-0.1502915031071255</v>
       </c>
       <c r="BD8">
-        <v>-6.7365115241807189E-2</v>
+        <v>-6.1581264028068863E-2</v>
       </c>
       <c r="BE8">
-        <v>6.9675427685334829E-2</v>
+        <v>5.7008599120724902E-2</v>
       </c>
       <c r="BF8">
-        <v>0.99274383279063028</v>
+        <v>0.93304124688352019</v>
       </c>
       <c r="BG8">
-        <v>0.99274383279063028</v>
+        <v>0.93304124688352019</v>
       </c>
       <c r="BH8" t="s">
+        <v>83</v>
+      </c>
+      <c r="BI8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
         <v>75</v>
       </c>
-      <c r="BI8" t="s">
-        <v>76</v>
+      <c r="E9">
+        <v>474380</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>474380</v>
+      </c>
+      <c r="J9">
+        <v>10075.113916</v>
+      </c>
+      <c r="K9">
+        <v>17819.351653167989</v>
+      </c>
+      <c r="L9">
+        <v>4.9174119999999997</v>
+      </c>
+      <c r="M9">
+        <v>2.4587059999999998</v>
+      </c>
+      <c r="N9">
+        <v>-0.13428699999999999</v>
+      </c>
+      <c r="O9">
+        <v>1.9375500000000001</v>
+      </c>
+      <c r="P9">
+        <v>2.123848795480416E-2</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0.19381293745909481</v>
+      </c>
+      <c r="S9">
+        <v>0.19264574056001521</v>
+      </c>
+      <c r="T9">
+        <v>2.1411866781904799E-2</v>
+      </c>
+      <c r="U9">
+        <v>4.1603708175563982E-4</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>5605</v>
+      </c>
+      <c r="Y9">
+        <v>468775</v>
+      </c>
+      <c r="Z9">
+        <v>2.405852167884379E-4</v>
+      </c>
+      <c r="AA9">
+        <v>7.6745872632113859E-3</v>
+      </c>
+      <c r="AB9">
+        <v>1.7774011741302409</v>
+      </c>
+      <c r="AC9">
+        <v>0.1228930196480815</v>
+      </c>
+      <c r="AD9">
+        <v>5605</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>3126</v>
+      </c>
+      <c r="AG9">
+        <v>1783</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>2.123848795480416E-2</v>
+      </c>
+      <c r="AM9">
+        <v>0.19264574056001521</v>
+      </c>
+      <c r="AN9">
+        <v>22065996167794.672</v>
+      </c>
+      <c r="AO9">
+        <v>1.33511954708937</v>
+      </c>
+      <c r="AP9">
+        <v>0.17288154152772159</v>
+      </c>
+      <c r="AQ9">
+        <v>-0.1342871479676091</v>
+      </c>
+      <c r="AR9">
+        <v>-7.28953018866626E-2</v>
+      </c>
+      <c r="AS9">
+        <v>1.291372016835211</v>
+      </c>
+      <c r="AT9">
+        <v>1927757557288.969</v>
+      </c>
+      <c r="AU9">
+        <v>9.0700655090501279</v>
+      </c>
+      <c r="AV9">
+        <v>80.601161473256838</v>
+      </c>
+      <c r="AW9">
+        <v>1.8443020363421731E-2</v>
+      </c>
+      <c r="AX9">
+        <v>0.98811501328049245</v>
+      </c>
+      <c r="AY9">
+        <v>1.9375500000000001</v>
+      </c>
+      <c r="AZ9">
+        <v>2.123848795480416E-2</v>
+      </c>
+      <c r="BA9">
+        <v>0.98155697963657829</v>
+      </c>
+      <c r="BC9">
+        <v>0.21784493839642791</v>
+      </c>
+      <c r="BD9">
+        <v>-0.35634716354282558</v>
+      </c>
+      <c r="BE9">
+        <v>0.39882413945243389</v>
+      </c>
+      <c r="BF9">
+        <v>0.98155697963657829</v>
+      </c>
+      <c r="BG9">
+        <v>0.98155697963657829</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>86</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to simple main with inputs
</commit_message>
<xml_diff>
--- a/src/m3c2_stats_all.xlsx
+++ b/src/m3c2_stats_all.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI11"/>
+  <dimension ref="A1:BI13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2648,6 +2648,388 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-08-20 13:13:44</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>data\rocks</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>474380</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>474380</v>
+      </c>
+      <c r="J12" t="n">
+        <v>10075.113916</v>
+      </c>
+      <c r="K12" t="n">
+        <v>17819.35165316799</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4.917412</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2.458706</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-0.134287</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1.93755</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.02123848795480416</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.1938129374590948</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.1926457405600152</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.0214118667819048</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.0004160370817556398</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>5605</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>468775</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.0002405852167884379</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.007674587263211386</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>1.777401174130241</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.1228930196480815</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>5605</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>3126</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>1783</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0.02123848795480416</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>0.1926457405600152</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>22065996167794.67</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>1.33511954708937</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>0.1728815415277216</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>-0.1342871479676091</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>-0.0728953018866626</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>1.291372016835211</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>1927757557288.969</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>9.070065509050128</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>80.60116147325684</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.01844302036342173</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9881150132804924</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>1.93755</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.02123848795480416</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>0.9815569796365783</v>
+      </c>
+      <c r="BB12" t="inlineStr"/>
+      <c r="BC12" t="n">
+        <v>0.2178449383964279</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>-0.3563471635428256</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>0.3988241394524339</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>0.9815569796365783</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>0.9815569796365783</v>
+      </c>
+      <c r="BH12" t="inlineStr">
+        <is>
+          <t>data\rocks\CC_points_zshift_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BI12" t="inlineStr">
+        <is>
+          <t>data\rocks\CC_points_zshift_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-08-20 13:17:56</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>data\rocks</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>474380</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>474380</v>
+      </c>
+      <c r="J13" t="n">
+        <v>10075.113916</v>
+      </c>
+      <c r="K13" t="n">
+        <v>17819.35165316799</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4.917412</v>
+      </c>
+      <c r="M13" t="n">
+        <v>2.458706</v>
+      </c>
+      <c r="N13" t="n">
+        <v>-0.134287</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1.93755</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.02123848795480416</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.1938129374590948</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.1926457405600152</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.0214118667819048</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.0004160370817556398</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>5605</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>468775</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.0002405852167884379</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.007674587263211386</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>1.777401174130241</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.1228930196480815</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>5605</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>3126</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>1783</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>0.02123848795480416</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>0.1926457405600152</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>22065996167794.67</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>1.33511954708937</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0.1728815415277216</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>-0.1342871479676091</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>-0.0728953018866626</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>1.291372016835211</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>1927757557288.969</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>9.070065509050128</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>80.60116147325684</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>0.01844302036342173</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>0.9881150132804924</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>1.93755</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>0.02123848795480416</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>0.9815569796365783</v>
+      </c>
+      <c r="BB13" t="inlineStr"/>
+      <c r="BC13" t="n">
+        <v>0.2178449383964279</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>-0.3563471635428256</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>0.3988241394524339</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>0.9815569796365783</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>0.9815569796365783</v>
+      </c>
+      <c r="BH13" t="inlineStr">
+        <is>
+          <t>data\rocks\CC_points_zshift_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BI13" t="inlineStr">
+        <is>
+          <t>data\rocks\CC_points_zshift_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>